<commit_message>
May 23 Take 3
</commit_message>
<xml_diff>
--- a/MSV000086809/sdrf.xlsx
+++ b/MSV000086809/sdrf.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eilenora\TMT_QC\MSV000086809\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\Payne Lab\TMT\TMT_QC\MSV000086809\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB2FA72-AB53-48B0-AE3D-B76DBF805531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E61A2A-290C-4232-926B-0CCC7B647973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6C6CB8E1-1F97-4EF2-94D7-A33AD26F6A9C}"/>
   </bookViews>
@@ -44,9 +44,6 @@
     <t>condition</t>
   </si>
   <si>
-    <t>f.MSV000086809/peak/Peak_List_Files/SingleCells/CellenONE_I3T_NEM_SC_Chip1_C1.mzML</t>
-  </si>
-  <si>
     <t>Plex</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>murine_mixture</t>
+  </si>
+  <si>
+    <t>CellenONE_I3T_NEM_SC_Chip1_C1.raw</t>
   </si>
 </sst>
 </file>
@@ -504,7 +504,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,36 +525,39 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="C2">
+        <v>16</v>
       </c>
       <c r="D2" s="1">
         <v>126</v>
@@ -563,13 +566,13 @@
         <v>126</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G2">
         <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -577,28 +580,31 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -606,28 +612,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -635,28 +644,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="C5">
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -664,28 +676,31 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="C6">
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -693,28 +708,31 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="C7">
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -722,28 +740,31 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="C8">
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -751,28 +772,31 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9" t="s">
-        <v>33</v>
-      </c>
       <c r="I9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -780,28 +804,31 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="C10">
+        <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -809,28 +836,31 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="C11">
+        <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -838,28 +868,31 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12">
+        <v>16</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12" t="s">
-        <v>33</v>
-      </c>
       <c r="I12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -867,28 +900,31 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="C13">
+        <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -896,28 +932,31 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="C14">
+        <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -925,28 +964,31 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15">
+        <v>16</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15" t="s">
-        <v>33</v>
-      </c>
       <c r="I15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J15">
         <v>1</v>
@@ -954,28 +996,31 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="C16">
+        <v>16</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -983,28 +1028,31 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J17">
         <v>1</v>

</xml_diff>